<commit_message>
Formated all files as PEP8 (PEP275) recomended, add input validation and add working examples in readme.
Formated all files with PEP8 recomidtation, add input data validation at
main module, and add exaples of work at readme file.
</commit_message>
<xml_diff>
--- a/project_folder/DZ_2.xlsx
+++ b/project_folder/DZ_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
@@ -201,15 +201,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>219075</xdr:colOff>
+          <xdr:colOff>220980</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>180975</xdr:colOff>
+          <xdr:colOff>182880</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -237,23 +237,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -553,13 +540,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,15 +561,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
+                <xdr:colOff>220980</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>180975</xdr:colOff>
+                <xdr:colOff>182880</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>30480</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -604,13 +591,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -626,7 +613,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -634,7 +621,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -642,7 +629,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -650,7 +637,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -658,7 +645,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -674,103 +661,103 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -784,16 +771,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -801,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -809,7 +796,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -817,7 +804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -825,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -833,7 +820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -854,13 +841,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -868,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -876,7 +863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -884,7 +871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -892,7 +879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -900,7 +887,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -921,14 +908,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -939,7 +926,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -950,7 +937,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
@@ -961,7 +948,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
@@ -972,7 +959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>

</xml_diff>